<commit_message>
update script and dashboard
</commit_message>
<xml_diff>
--- a/misc/hcris_shiny_variables.xlsx
+++ b/misc/hcris_shiny_variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Dropbox\Projects\costreports\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfang\Dropbox\Projects\costreports\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
   <si>
     <t>variable</t>
   </si>
@@ -318,10 +318,28 @@
     <t>Financial margin for all hospital activities</t>
   </si>
   <si>
-    <t>Revenue collected by the hospital for patient care after payer discounts (not charges)</t>
-  </si>
-  <si>
     <t>Financial margin for patient care activities across all payers</t>
+  </si>
+  <si>
+    <t>Operating Expense</t>
+  </si>
+  <si>
+    <t>Nonoperating Revenue</t>
+  </si>
+  <si>
+    <t>Revenue collected by the hospital for inpatient and outpatient care after payer discounts (actual payments, not charges)</t>
+  </si>
+  <si>
+    <t>Revenue collected by the hospital for activities other than patient care (i.e., investment income)</t>
+  </si>
+  <si>
+    <t>Expenses paid by the hospital for patient care activities</t>
+  </si>
+  <si>
+    <t>Worksheet G3, column 1, line 25</t>
+  </si>
+  <si>
+    <t>Worksheet G3, column 1, line 4</t>
   </si>
 </sst>
 </file>
@@ -357,8 +375,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,12 +664,12 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -690,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -707,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -724,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -741,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -758,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -775,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -792,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -809,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -826,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -843,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -860,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -877,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -894,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -911,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -928,7 +947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -945,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -962,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -979,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -996,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1013,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1030,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1047,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1064,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1098,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1122,20 +1141,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C19" sqref="A1:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="109" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1146,7 +1165,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1157,7 +1176,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1168,7 +1187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1179,7 +1198,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1190,7 +1209,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1201,126 +1220,154 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B14" t="s">
         <v>96</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
         <v>97</v>
       </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>77</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>72</v>
       </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:C17">

</xml_diff>